<commit_message>
Subiendo Casos de Pruebas y documentacion con link a notion
</commit_message>
<xml_diff>
--- a/Casos de Prueba US - NomadaX.xlsx
+++ b/Casos de Prueba US - NomadaX.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Casos de Prueba Profesionales" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sprint I" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sprint II" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="D+46JgOHH90bEPxSSvAvUF27SaysN5qh025qEvF/LqU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="2a1lgfpTzpoDgPUFMdzmjQ3KsYsL0XWjg7Hlsa/WUos="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="209">
   <si>
     <t>ID Historia</t>
   </si>
@@ -375,6 +376,279 @@
   </si>
   <si>
     <t>No se realizan cambios</t>
+  </si>
+  <si>
+    <t>H12</t>
+  </si>
+  <si>
+    <t>Categorizar productos</t>
+  </si>
+  <si>
+    <t>H12-TC01</t>
+  </si>
+  <si>
+    <t>Asignar categoría al crear producto</t>
+  </si>
+  <si>
+    <t>Asignar categoría desde formulario de nuevo producto</t>
+  </si>
+  <si>
+    <t>Categoría asignada y visible</t>
+  </si>
+  <si>
+    <t>✅ Ejecutado exitosamente</t>
+  </si>
+  <si>
+    <t>H12-TC02</t>
+  </si>
+  <si>
+    <t>Editar producto y cambiar categoría</t>
+  </si>
+  <si>
+    <t>Editar producto, cambiar categoría</t>
+  </si>
+  <si>
+    <t>Nueva categoría guardada y visible</t>
+  </si>
+  <si>
+    <t>H13</t>
+  </si>
+  <si>
+    <t>Registrar usuario</t>
+  </si>
+  <si>
+    <t>H13-TC01</t>
+  </si>
+  <si>
+    <t>Registro con datos válidos</t>
+  </si>
+  <si>
+    <t>Registrar usuario con campos válidos</t>
+  </si>
+  <si>
+    <t>Usuario creado correctamente</t>
+  </si>
+  <si>
+    <t>H13-TC02</t>
+  </si>
+  <si>
+    <t>Campos vacíos o inválidos</t>
+  </si>
+  <si>
+    <t>Probar validación en campos vacíos o erróneos</t>
+  </si>
+  <si>
+    <t>Errores mostrados, no se registra</t>
+  </si>
+  <si>
+    <t>H14</t>
+  </si>
+  <si>
+    <t>Identificar usuario</t>
+  </si>
+  <si>
+    <t>H14-TC01</t>
+  </si>
+  <si>
+    <t>Login exitoso</t>
+  </si>
+  <si>
+    <t>Iniciar sesión con credenciales válidas</t>
+  </si>
+  <si>
+    <t>Usuario autenticado con avatar visible</t>
+  </si>
+  <si>
+    <t>H14-TC02</t>
+  </si>
+  <si>
+    <t>Login fallido</t>
+  </si>
+  <si>
+    <t>Intentar login con datos incorrectos</t>
+  </si>
+  <si>
+    <t>Mensaje de error visible</t>
+  </si>
+  <si>
+    <t>H15</t>
+  </si>
+  <si>
+    <t>Cerrar sesión</t>
+  </si>
+  <si>
+    <t>H15-TC01</t>
+  </si>
+  <si>
+    <t>Cerrar sesión correctamente</t>
+  </si>
+  <si>
+    <t>Click en 'Cerrar sesión'</t>
+  </si>
+  <si>
+    <t>Sesión cerrada, vuelve a estado anónimo</t>
+  </si>
+  <si>
+    <t>H16</t>
+  </si>
+  <si>
+    <t>Identificar administrador</t>
+  </si>
+  <si>
+    <t>H16-TC01</t>
+  </si>
+  <si>
+    <t>Asignar rol de administrador</t>
+  </si>
+  <si>
+    <t>Desde panel, asignar o quitar rol</t>
+  </si>
+  <si>
+    <t>Rol actualizado correctamente</t>
+  </si>
+  <si>
+    <t>H16-TC02</t>
+  </si>
+  <si>
+    <t>Verificación de permisos</t>
+  </si>
+  <si>
+    <t>Probar accesos con diferentes roles</t>
+  </si>
+  <si>
+    <t>Permisos aplicados según rol</t>
+  </si>
+  <si>
+    <t>H17</t>
+  </si>
+  <si>
+    <t>Administrar características</t>
+  </si>
+  <si>
+    <t>H17-TC01</t>
+  </si>
+  <si>
+    <t>Crear nueva característica</t>
+  </si>
+  <si>
+    <t>Añadir característica con nombre e ícono</t>
+  </si>
+  <si>
+    <t>Característica visible en el listado</t>
+  </si>
+  <si>
+    <t>H17-TC02</t>
+  </si>
+  <si>
+    <t>Editar/eliminar característica</t>
+  </si>
+  <si>
+    <t>Modificar o eliminar característica</t>
+  </si>
+  <si>
+    <t>Cambios reflejados</t>
+  </si>
+  <si>
+    <t>H18</t>
+  </si>
+  <si>
+    <t>Visualizar características</t>
+  </si>
+  <si>
+    <t>H18-TC01</t>
+  </si>
+  <si>
+    <t>Ver características en detalle</t>
+  </si>
+  <si>
+    <t>Ver sección de características en producto</t>
+  </si>
+  <si>
+    <t>Características con íconos visibles</t>
+  </si>
+  <si>
+    <t>H19</t>
+  </si>
+  <si>
+    <t>Confirmación de registro</t>
+  </si>
+  <si>
+    <t>H19-TC01</t>
+  </si>
+  <si>
+    <t>Email tras registro</t>
+  </si>
+  <si>
+    <t>Registrarse y esperar correo</t>
+  </si>
+  <si>
+    <t>Email de bienvenida recibido</t>
+  </si>
+  <si>
+    <t>❌ No implementado aún</t>
+  </si>
+  <si>
+    <t>#19 - Confirmación de registro</t>
+  </si>
+  <si>
+    <t>H19-TC02</t>
+  </si>
+  <si>
+    <t>Reenviar email</t>
+  </si>
+  <si>
+    <t>Click en opción para reenviar</t>
+  </si>
+  <si>
+    <t>Email reenviado correctamente</t>
+  </si>
+  <si>
+    <t>H20</t>
+  </si>
+  <si>
+    <t>Crear sección de categorías</t>
+  </si>
+  <si>
+    <t>H20-TC01</t>
+  </si>
+  <si>
+    <t>Filtrar por categorías</t>
+  </si>
+  <si>
+    <t>Seleccionar una o más categorías</t>
+  </si>
+  <si>
+    <t>Productos filtrados correctamente</t>
+  </si>
+  <si>
+    <t>H20-TC02</t>
+  </si>
+  <si>
+    <t>Borrar filtros</t>
+  </si>
+  <si>
+    <t>Quitar filtros aplicados</t>
+  </si>
+  <si>
+    <t>Lista vuelve a mostrar todo</t>
+  </si>
+  <si>
+    <t>H21</t>
+  </si>
+  <si>
+    <t>Agregar categoría</t>
+  </si>
+  <si>
+    <t>H21-TC01</t>
+  </si>
+  <si>
+    <t>Crear nueva categoría</t>
+  </si>
+  <si>
+    <t>Agregar categoría con título, descripción e imagen</t>
+  </si>
+  <si>
+    <t>Categoría aparece correctamente</t>
   </si>
 </sst>
 </file>
@@ -400,7 +674,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,6 +753,42 @@
         <bgColor rgb="FFF9CB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAD1DC"/>
+        <bgColor rgb="FFEAD1DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D2E9"/>
+        <bgColor rgb="FFD9D2E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAE9C8"/>
+        <bgColor rgb="FFEAE9C8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border/>
@@ -500,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -545,6 +855,96 @@
     </xf>
     <xf borderId="1" fillId="13" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="14" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="14" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="14" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="15" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="15" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="15" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="16" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="16" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="16" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="17" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="17" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="17" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="18" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="18" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="18" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="19" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="19" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="19" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,6 +955,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2284,4 +2688,441 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="18.71"/>
+    <col customWidth="1" min="2" max="2" width="32.57"/>
+    <col customWidth="1" min="4" max="4" width="44.71"/>
+    <col customWidth="1" min="5" max="5" width="48.86"/>
+    <col customWidth="1" min="6" max="6" width="35.86"/>
+    <col customWidth="1" min="7" max="7" width="29.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="40.5" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" ht="24.0" customHeight="1">
+      <c r="A2" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" ht="24.0" customHeight="1">
+      <c r="A3" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" ht="24.0" customHeight="1">
+      <c r="A4" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" ht="24.0" customHeight="1">
+      <c r="A5" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" ht="24.0" customHeight="1">
+      <c r="A6" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" ht="24.0" customHeight="1">
+      <c r="A7" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" ht="24.0" customHeight="1">
+      <c r="A8" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" ht="24.0" customHeight="1">
+      <c r="A9" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" ht="24.0" customHeight="1">
+      <c r="A10" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" ht="24.0" customHeight="1">
+      <c r="A11" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" ht="24.0" customHeight="1">
+      <c r="A12" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" ht="24.0" customHeight="1">
+      <c r="A13" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" ht="24.0" customHeight="1">
+      <c r="A14" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" ht="24.0" customHeight="1">
+      <c r="A15" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="F15" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" ht="24.0" customHeight="1">
+      <c r="A16" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" ht="24.0" customHeight="1">
+      <c r="A17" s="39" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" ht="24.0" customHeight="1">
+      <c r="A18" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>208</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Subiendo casos de prueba excel
</commit_message>
<xml_diff>
--- a/Casos de Prueba US - NomadaX.xlsx
+++ b/Casos de Prueba US - NomadaX.xlsx
@@ -5,19 +5,20 @@
   <sheets>
     <sheet state="visible" name="Sprint I" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Sprint II" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Hoja 2" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="2a1lgfpTzpoDgPUFMdzmjQ3KsYsL0XWjg7Hlsa/WUos="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="pFLE3r6wbsoaukTOSs6gpqxWLSLX1XDzGqY052UVdGo="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="273">
   <si>
     <t>ID Historia</t>
   </si>
@@ -649,13 +650,205 @@
   </si>
   <si>
     <t>Categoría aparece correctamente</t>
+  </si>
+  <si>
+    <t>H22</t>
+  </si>
+  <si>
+    <t>Realizar búsqueda</t>
+  </si>
+  <si>
+    <t>H22-TC01</t>
+  </si>
+  <si>
+    <t>Buscar productos con criterios válidos</t>
+  </si>
+  <si>
+    <t>Ingresar título, fechas, hacer clic en "Realizar búsqueda"</t>
+  </si>
+  <si>
+    <t>Productos mostrados con secciones visibles</t>
+  </si>
+  <si>
+    <t>H22-TC02</t>
+  </si>
+  <si>
+    <t>Autocompletado de búsqueda</t>
+  </si>
+  <si>
+    <t>Escribir en campo de búsqueda</t>
+  </si>
+  <si>
+    <t>Sugerencias visibles y seleccionables</t>
+  </si>
+  <si>
+    <t>H23</t>
+  </si>
+  <si>
+    <t>Visualizar disponibilidad</t>
+  </si>
+  <si>
+    <t>H23-TC01</t>
+  </si>
+  <si>
+    <t>Mostrar disponibilidad en calendario</t>
+  </si>
+  <si>
+    <t>Abrir ficha del producto</t>
+  </si>
+  <si>
+    <t>Fechas ocupadas y libres claramente diferenciadas</t>
+  </si>
+  <si>
+    <t>H23-TC02</t>
+  </si>
+  <si>
+    <t>Manejo de errores de disponibilidad</t>
+  </si>
+  <si>
+    <t>Simular error en backend o conexión</t>
+  </si>
+  <si>
+    <t>Mensaje de error visible sin afectar el resto del contenido</t>
+  </si>
+  <si>
+    <t>H24</t>
+  </si>
+  <si>
+    <t>Marcar como favorito</t>
+  </si>
+  <si>
+    <t>H24-TC01</t>
+  </si>
+  <si>
+    <t>Añadir producto a favoritos</t>
+  </si>
+  <si>
+    <t>Clic en ícono de favorito</t>
+  </si>
+  <si>
+    <t>Producto marcado correctamente</t>
+  </si>
+  <si>
+    <t>H24-TC02</t>
+  </si>
+  <si>
+    <t>Quitar producto de favoritos</t>
+  </si>
+  <si>
+    <t>Clic nuevamente en el ícono</t>
+  </si>
+  <si>
+    <t>Producto eliminado de favoritos</t>
+  </si>
+  <si>
+    <t>H25</t>
+  </si>
+  <si>
+    <t>Listar productos favoritos</t>
+  </si>
+  <si>
+    <t>H25-TC01</t>
+  </si>
+  <si>
+    <t>Ver lista de favoritos</t>
+  </si>
+  <si>
+    <t>Acceder desde cuenta del usuario</t>
+  </si>
+  <si>
+    <t>Productos favoritos listados correctamente</t>
+  </si>
+  <si>
+    <t>H25-TC02</t>
+  </si>
+  <si>
+    <t>Eliminar desde lista</t>
+  </si>
+  <si>
+    <t>Clic en eliminar en un producto favorito</t>
+  </si>
+  <si>
+    <t>Producto eliminado de la lista</t>
+  </si>
+  <si>
+    <t>H26</t>
+  </si>
+  <si>
+    <t>Ver bloque de políticas</t>
+  </si>
+  <si>
+    <t>H26-TC01</t>
+  </si>
+  <si>
+    <t>Mostrar políticas del producto</t>
+  </si>
+  <si>
+    <t>Abrir ficha de producto</t>
+  </si>
+  <si>
+    <t>Bloque visible con columnas, título y descripciones</t>
+  </si>
+  <si>
+    <t>H27</t>
+  </si>
+  <si>
+    <t>Compartir productos</t>
+  </si>
+  <si>
+    <t>H27-TC01</t>
+  </si>
+  <si>
+    <t>Compartir en redes sociales</t>
+  </si>
+  <si>
+    <t>Clic en "Compartir", seleccionar red, escribir mensaje</t>
+  </si>
+  <si>
+    <t>Contenido compartido correctamente</t>
+  </si>
+  <si>
+    <t>H28</t>
+  </si>
+  <si>
+    <t>Puntuar producto</t>
+  </si>
+  <si>
+    <t>H28-TC01</t>
+  </si>
+  <si>
+    <t>Enviar puntuación tras reserva</t>
+  </si>
+  <si>
+    <t>Usuario califica con estrellas y comentario</t>
+  </si>
+  <si>
+    <t>Puntuación visible con nombre, fecha y media actualizada</t>
+  </si>
+  <si>
+    <t>H29</t>
+  </si>
+  <si>
+    <t>Eliminar categoría</t>
+  </si>
+  <si>
+    <t>H29-TC01</t>
+  </si>
+  <si>
+    <t>Eliminar una categoría desde el panel</t>
+  </si>
+  <si>
+    <t>Clic en eliminar, confirmar acción</t>
+  </si>
+  <si>
+    <t>Categoría eliminada, mensaje de confirmación mostrado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -673,8 +866,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -789,6 +987,18 @@
         <bgColor rgb="FFEAE9C8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA2C4C9"/>
+        <bgColor rgb="FFA2C4C9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA9999"/>
+        <bgColor rgb="FFEA9999"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border/>
@@ -810,7 +1020,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="54">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -945,6 +1155,33 @@
     </xf>
     <xf borderId="1" fillId="19" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="20" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="21" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -959,6 +1196,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -3125,4 +3366,327 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="10.29"/>
+    <col customWidth="1" min="2" max="2" width="22.71"/>
+    <col customWidth="1" min="3" max="3" width="9.43"/>
+    <col customWidth="1" min="4" max="4" width="33.29"/>
+    <col customWidth="1" min="5" max="5" width="48.71"/>
+    <col customWidth="1" min="6" max="6" width="50.14"/>
+    <col customWidth="1" min="7" max="7" width="24.86"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="29.25" customHeight="1">
+      <c r="A1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" ht="29.25" customHeight="1">
+      <c r="A2" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>214</v>
+      </c>
+      <c r="G2" s="46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" ht="29.25" customHeight="1">
+      <c r="A3" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" ht="29.25" customHeight="1">
+      <c r="A4" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" ht="29.25" customHeight="1">
+      <c r="A5" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="G5" s="47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" ht="29.25" customHeight="1">
+      <c r="A6" s="48" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>231</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="F6" s="48" t="s">
+        <v>234</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" ht="29.25" customHeight="1">
+      <c r="A7" s="48" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>230</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="G7" s="48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" ht="29.25" customHeight="1">
+      <c r="A8" s="49" t="s">
+        <v>239</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>240</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>241</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>242</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>244</v>
+      </c>
+      <c r="G8" s="49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" ht="29.25" customHeight="1">
+      <c r="A9" s="49" t="s">
+        <v>239</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>240</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>245</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>246</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>247</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>248</v>
+      </c>
+      <c r="G9" s="49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" ht="29.25" customHeight="1">
+      <c r="A10" s="50" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>252</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>253</v>
+      </c>
+      <c r="F10" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="G10" s="50" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" ht="29.25" customHeight="1">
+      <c r="A11" s="51" t="s">
+        <v>255</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>257</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>258</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>259</v>
+      </c>
+      <c r="F11" s="51" t="s">
+        <v>260</v>
+      </c>
+      <c r="G11" s="51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" ht="29.25" customHeight="1">
+      <c r="A12" s="52" t="s">
+        <v>261</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>262</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>263</v>
+      </c>
+      <c r="D12" s="52" t="s">
+        <v>264</v>
+      </c>
+      <c r="E12" s="52" t="s">
+        <v>265</v>
+      </c>
+      <c r="F12" s="52" t="s">
+        <v>266</v>
+      </c>
+      <c r="G12" s="52" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" ht="29.25" customHeight="1">
+      <c r="A13" s="53" t="s">
+        <v>267</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>268</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>269</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>272</v>
+      </c>
+      <c r="G13" s="53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Subiendo excel con las pruebas
</commit_message>
<xml_diff>
--- a/Casos de Prueba US - NomadaX.xlsx
+++ b/Casos de Prueba US - NomadaX.xlsx
@@ -5,20 +5,21 @@
   <sheets>
     <sheet state="visible" name="Sprint I" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Sprint II" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Hoja 2" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Sprint III" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Sprint IV" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="pFLE3r6wbsoaukTOSs6gpqxWLSLX1XDzGqY052UVdGo="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="0hmNgIEfc91ogH8cU/IgidzQ6Dkblay69ZhxDzOhSlA="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="361">
   <si>
     <t>ID Historia</t>
   </si>
@@ -842,6 +843,270 @@
   </si>
   <si>
     <t>Categoría eliminada, mensaje de confirmación mostrado</t>
+  </si>
+  <si>
+    <t>H30</t>
+  </si>
+  <si>
+    <t>Reservas – Seleccionar fecha</t>
+  </si>
+  <si>
+    <t>H30-TC01</t>
+  </si>
+  <si>
+    <t>Acceso desde detalle del producto</t>
+  </si>
+  <si>
+    <t>Ir a detalle del producto, hacer clic en “Reservar”</t>
+  </si>
+  <si>
+    <t>Redirección correcta a sección de reservas si está logueado</t>
+  </si>
+  <si>
+    <t>H30-TC02</t>
+  </si>
+  <si>
+    <t>Redirección si no está logueado</t>
+  </si>
+  <si>
+    <t>Clic en “Reservar” sin sesión iniciada</t>
+  </si>
+  <si>
+    <t>Redirección a login con mensaje claro</t>
+  </si>
+  <si>
+    <t>H30-TC03</t>
+  </si>
+  <si>
+    <t>Buscar productos disponibles por fecha</t>
+  </si>
+  <si>
+    <t>Ingresar rango de fechas y buscar</t>
+  </si>
+  <si>
+    <t>Lista con productos disponibles mostrada correctamente</t>
+  </si>
+  <si>
+    <t>H30-TC04</t>
+  </si>
+  <si>
+    <t>Validación de fechas ocupadas</t>
+  </si>
+  <si>
+    <t>Seleccionar fechas ocupadas y hacer búsqueda</t>
+  </si>
+  <si>
+    <t>Mensaje de advertencia o bloqueo de selección</t>
+  </si>
+  <si>
+    <t>H31</t>
+  </si>
+  <si>
+    <t>Reservas – Visualizar detalles</t>
+  </si>
+  <si>
+    <t>H31-TC01</t>
+  </si>
+  <si>
+    <t>Visualización completa del producto</t>
+  </si>
+  <si>
+    <t>Acceder al resumen antes de reservar</t>
+  </si>
+  <si>
+    <t>Información detallada del producto visible</t>
+  </si>
+  <si>
+    <t>H31-TC02</t>
+  </si>
+  <si>
+    <t>Mostrar datos del usuario</t>
+  </si>
+  <si>
+    <t>Iniciar sesión, acceder a reservas</t>
+  </si>
+  <si>
+    <t>Nombre, email y otros datos mostrados</t>
+  </si>
+  <si>
+    <t>H31-TC03</t>
+  </si>
+  <si>
+    <t>Visualización del periodo seleccionado</t>
+  </si>
+  <si>
+    <t>Seleccionar fechas, avanzar a confirmación</t>
+  </si>
+  <si>
+    <t>Fechas claramente mostradas en pantalla</t>
+  </si>
+  <si>
+    <t>H31-TC04</t>
+  </si>
+  <si>
+    <t>Confirmar la reserva desde la vista</t>
+  </si>
+  <si>
+    <t>Clic en botón “Confirmar reserva”</t>
+  </si>
+  <si>
+    <t>Reserva enviada con éxito</t>
+  </si>
+  <si>
+    <t>H32</t>
+  </si>
+  <si>
+    <t>Realizar reserva</t>
+  </si>
+  <si>
+    <t>H32-TC01</t>
+  </si>
+  <si>
+    <t>Seleccionar producto y fechas válidas</t>
+  </si>
+  <si>
+    <t>Elegir producto y fechas disponibles</t>
+  </si>
+  <si>
+    <t>Continuar al siguiente paso de reserva</t>
+  </si>
+  <si>
+    <t>H32-TC02</t>
+  </si>
+  <si>
+    <t>Visualizar campos opcionales</t>
+  </si>
+  <si>
+    <t>Iniciar reserva y revisar el formulario</t>
+  </si>
+  <si>
+    <t>Campos adicionales visibles y editables</t>
+  </si>
+  <si>
+    <t>H32-TC03</t>
+  </si>
+  <si>
+    <t>Confirmación de reserva</t>
+  </si>
+  <si>
+    <t>Completar formulario y confirmar</t>
+  </si>
+  <si>
+    <t>Página de confirmación mostrada</t>
+  </si>
+  <si>
+    <t>H32-TC04</t>
+  </si>
+  <si>
+    <t>Manejo de errores</t>
+  </si>
+  <si>
+    <t>Simular fallo (campo vacío o fechas incorrectas)</t>
+  </si>
+  <si>
+    <t>Mensaje de error claro y no disruptivo</t>
+  </si>
+  <si>
+    <t>H33</t>
+  </si>
+  <si>
+    <t>Acceder a historial de reservas</t>
+  </si>
+  <si>
+    <t>H33-TC01</t>
+  </si>
+  <si>
+    <t>Ver historial de reservas</t>
+  </si>
+  <si>
+    <t>Acceder a sección de historial</t>
+  </si>
+  <si>
+    <t>Lista ordenada con datos del producto, fecha y uso</t>
+  </si>
+  <si>
+    <t>H34</t>
+  </si>
+  <si>
+    <t>WhatsApp – Iniciar chat</t>
+  </si>
+  <si>
+    <t>H34-TC01</t>
+  </si>
+  <si>
+    <t>Botón WhatsApp visible y funcional</t>
+  </si>
+  <si>
+    <t>Ver página del producto en móvil o PC, buscar ícono de WhatsApp</t>
+  </si>
+  <si>
+    <t>Botón siempre visible, clic abre WhatsApp con mensaje predefinido</t>
+  </si>
+  <si>
+    <t>H34-TC02</t>
+  </si>
+  <si>
+    <t>Enviar mensaje sin login</t>
+  </si>
+  <si>
+    <t>Sin iniciar sesión, usar botón WhatsApp</t>
+  </si>
+  <si>
+    <t>Envío exitoso, sin requerir autenticación</t>
+  </si>
+  <si>
+    <t>H34-TC03</t>
+  </si>
+  <si>
+    <t>Manejo de errores de envío</t>
+  </si>
+  <si>
+    <t>Simular error en red o número incorrecto</t>
+  </si>
+  <si>
+    <t>Mostrar mensaje de error sin afectar el resto del contenido</t>
+  </si>
+  <si>
+    <t>H35</t>
+  </si>
+  <si>
+    <t>Confirmar reserva por correo</t>
+  </si>
+  <si>
+    <t>H35-TC01</t>
+  </si>
+  <si>
+    <t>Envío automático tras reserva</t>
+  </si>
+  <si>
+    <t>Realizar una reserva</t>
+  </si>
+  <si>
+    <t>Email llega automáticamente con datos correctos</t>
+  </si>
+  <si>
+    <t>H35-TC02</t>
+  </si>
+  <si>
+    <t>Visualización correcta en todos los dispositivos</t>
+  </si>
+  <si>
+    <t>Abrir correo desde diferentes dispositivos</t>
+  </si>
+  <si>
+    <t>Diseño adaptado y legible</t>
+  </si>
+  <si>
+    <t>H35-TC03</t>
+  </si>
+  <si>
+    <t>Entrega en menos de 24h</t>
+  </si>
+  <si>
+    <t>Reservar y verificar bandeja de entrada en las horas siguientes</t>
+  </si>
+  <si>
+    <t>Correo recibido en plazo indicado</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1285,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1181,6 +1446,27 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="15" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1200,6 +1486,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -3689,4 +3979,487 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="28.86"/>
+    <col customWidth="1" min="3" max="3" width="12.29"/>
+    <col customWidth="1" min="4" max="4" width="42.57"/>
+    <col customWidth="1" min="5" max="5" width="57.14"/>
+    <col customWidth="1" min="6" max="6" width="58.43"/>
+    <col customWidth="1" min="7" max="7" width="24.86"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="31.5" customHeight="1">
+      <c r="A1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="55" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>274</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>275</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>277</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>278</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="55" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>280</v>
+      </c>
+      <c r="E3" s="55" t="s">
+        <v>281</v>
+      </c>
+      <c r="F3" s="55" t="s">
+        <v>282</v>
+      </c>
+      <c r="G3" s="55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="55" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>283</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>284</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>285</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>286</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="55" t="s">
+        <v>273</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>287</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>288</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>289</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>290</v>
+      </c>
+      <c r="G5" s="55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" ht="18.75" customHeight="1">
+      <c r="A6" s="56" t="s">
+        <v>291</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>292</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>293</v>
+      </c>
+      <c r="D6" s="56" t="s">
+        <v>294</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>295</v>
+      </c>
+      <c r="F6" s="56" t="s">
+        <v>296</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" ht="18.75" customHeight="1">
+      <c r="A7" s="56" t="s">
+        <v>291</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>292</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>297</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>298</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>299</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>300</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" ht="18.75" customHeight="1">
+      <c r="A8" s="56" t="s">
+        <v>291</v>
+      </c>
+      <c r="B8" s="56" t="s">
+        <v>292</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>301</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>302</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>303</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>304</v>
+      </c>
+      <c r="G8" s="56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" ht="18.75" customHeight="1">
+      <c r="A9" s="56" t="s">
+        <v>291</v>
+      </c>
+      <c r="B9" s="56" t="s">
+        <v>292</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>305</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>306</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>307</v>
+      </c>
+      <c r="F9" s="56" t="s">
+        <v>308</v>
+      </c>
+      <c r="G9" s="56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" ht="18.75" customHeight="1">
+      <c r="A10" s="57" t="s">
+        <v>309</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>310</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>311</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>312</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>313</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>314</v>
+      </c>
+      <c r="G10" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" ht="18.75" customHeight="1">
+      <c r="A11" s="57" t="s">
+        <v>309</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>310</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>315</v>
+      </c>
+      <c r="D11" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="E11" s="57" t="s">
+        <v>317</v>
+      </c>
+      <c r="F11" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="G11" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" ht="18.75" customHeight="1">
+      <c r="A12" s="57" t="s">
+        <v>309</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>310</v>
+      </c>
+      <c r="C12" s="57" t="s">
+        <v>319</v>
+      </c>
+      <c r="D12" s="57" t="s">
+        <v>320</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>321</v>
+      </c>
+      <c r="F12" s="57" t="s">
+        <v>322</v>
+      </c>
+      <c r="G12" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" ht="18.75" customHeight="1">
+      <c r="A13" s="57" t="s">
+        <v>309</v>
+      </c>
+      <c r="B13" s="57" t="s">
+        <v>310</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>323</v>
+      </c>
+      <c r="D13" s="57" t="s">
+        <v>324</v>
+      </c>
+      <c r="E13" s="57" t="s">
+        <v>325</v>
+      </c>
+      <c r="F13" s="57" t="s">
+        <v>326</v>
+      </c>
+      <c r="G13" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" ht="18.75" customHeight="1">
+      <c r="A14" s="58" t="s">
+        <v>327</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>328</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>329</v>
+      </c>
+      <c r="D14" s="58" t="s">
+        <v>330</v>
+      </c>
+      <c r="E14" s="58" t="s">
+        <v>331</v>
+      </c>
+      <c r="F14" s="58" t="s">
+        <v>332</v>
+      </c>
+      <c r="G14" s="58" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" ht="18.75" customHeight="1">
+      <c r="A15" s="59" t="s">
+        <v>333</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>334</v>
+      </c>
+      <c r="C15" s="59" t="s">
+        <v>335</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>336</v>
+      </c>
+      <c r="E15" s="59" t="s">
+        <v>337</v>
+      </c>
+      <c r="F15" s="59" t="s">
+        <v>338</v>
+      </c>
+      <c r="G15" s="59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" ht="18.75" customHeight="1">
+      <c r="A16" s="59" t="s">
+        <v>333</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>334</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>339</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>340</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>341</v>
+      </c>
+      <c r="F16" s="59" t="s">
+        <v>342</v>
+      </c>
+      <c r="G16" s="59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" ht="18.75" customHeight="1">
+      <c r="A17" s="59" t="s">
+        <v>333</v>
+      </c>
+      <c r="B17" s="59" t="s">
+        <v>334</v>
+      </c>
+      <c r="C17" s="59" t="s">
+        <v>343</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>344</v>
+      </c>
+      <c r="E17" s="59" t="s">
+        <v>345</v>
+      </c>
+      <c r="F17" s="59" t="s">
+        <v>346</v>
+      </c>
+      <c r="G17" s="59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" ht="18.75" customHeight="1">
+      <c r="A18" s="60" t="s">
+        <v>347</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>348</v>
+      </c>
+      <c r="C18" s="60" t="s">
+        <v>349</v>
+      </c>
+      <c r="D18" s="60" t="s">
+        <v>350</v>
+      </c>
+      <c r="E18" s="60" t="s">
+        <v>351</v>
+      </c>
+      <c r="F18" s="60" t="s">
+        <v>352</v>
+      </c>
+      <c r="G18" s="60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" ht="18.75" customHeight="1">
+      <c r="A19" s="60" t="s">
+        <v>347</v>
+      </c>
+      <c r="B19" s="60" t="s">
+        <v>348</v>
+      </c>
+      <c r="C19" s="60" t="s">
+        <v>353</v>
+      </c>
+      <c r="D19" s="60" t="s">
+        <v>354</v>
+      </c>
+      <c r="E19" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="F19" s="60" t="s">
+        <v>356</v>
+      </c>
+      <c r="G19" s="60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" ht="18.75" customHeight="1">
+      <c r="A20" s="60" t="s">
+        <v>347</v>
+      </c>
+      <c r="B20" s="60" t="s">
+        <v>348</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>357</v>
+      </c>
+      <c r="D20" s="60" t="s">
+        <v>358</v>
+      </c>
+      <c r="E20" s="60" t="s">
+        <v>359</v>
+      </c>
+      <c r="F20" s="60" t="s">
+        <v>360</v>
+      </c>
+      <c r="G20" s="60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>